<commit_message>
Auto-committed on 2022/12/14 週三 17:14:12.76
</commit_message>
<xml_diff>
--- a/Program/Other/銀扣失敗五萬元以上報表-底稿.xlsx
+++ b/Program/Other/銀扣失敗五萬元以上報表-底稿.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7580"/>
   </bookViews>
   <sheets>
     <sheet name="LAW7N1Ppp" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LAW7N1Ppp!$G$1:$G$1</definedName>
-    <definedName name="_xlnm.Database">LAW7N1Ppp!$A$1:$J$1</definedName>
+    <definedName name="_xlnm.Database">LAW7N1Ppp!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>帳號</t>
   </si>
@@ -50,6 +50,10 @@
   </si>
   <si>
     <t>地區別</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>地區別代號</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1027,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -1043,10 +1047,11 @@
     <col min="6" max="6" width="26.81640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.81640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1075,6 +1080,9 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>